<commit_message>
Implement stock and tag inputs
</commit_message>
<xml_diff>
--- a/notes_resources.xlsx
+++ b/notes_resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matts\dev10\finet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2013A429-D045-4F5E-A0D9-EA9E3D74D59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7926071-F2AF-4861-8002-87D5248CE23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>https://medium.com/geekculture/how-to-execute-a-rest-api-call-on-apache-spark-the-right-way-in-python-4367f2740e78</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>Connect to Alpha Vantage API</t>
+  </si>
+  <si>
+    <t>AV key</t>
+  </si>
+  <si>
+    <t>0IBANWKGCSZILWKU</t>
   </si>
 </sst>
 </file>
@@ -136,8 +142,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,6 +472,14 @@
       </c>
       <c r="B10" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -476,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2281EE47-97FB-48EC-8AF3-3870E558894B}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>